<commit_message>
adding citations network macro code
</commit_message>
<xml_diff>
--- a/data/raw/collected_metadata/metadata_citation.xlsx
+++ b/data/raw/collected_metadata/metadata_citation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://genes-my.sharepoint.com/personal/lmaurice_ensae_fr/Documents/CCNE/Analyse/CCNE/data/raw/collected_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1319" documentId="8_{348236E8-4DE9-42EE-8823-92D63E993468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F700E402-8C20-46AB-B686-55764DBF249B}"/>
+  <xr:revisionPtr revIDLastSave="1505" documentId="8_{348236E8-4DE9-42EE-8823-92D63E993468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99F98C94-724A-4DB3-8512-1875DB53CF8F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55944493-B888-42B6-8128-05B0549678CA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{55944493-B888-42B6-8128-05B0549678CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="532">
   <si>
     <t>citation_id</t>
   </si>
@@ -812,24 +812,6 @@
     <t>presse:lemonde:24012003</t>
   </si>
   <si>
-    <t>article;médical</t>
-  </si>
-  <si>
-    <t>livre;éthique</t>
-  </si>
-  <si>
-    <t>article;éthique</t>
-  </si>
-  <si>
-    <t>article;droit</t>
-  </si>
-  <si>
-    <t>thèse;SHS</t>
-  </si>
-  <si>
-    <t>article;bio</t>
-  </si>
-  <si>
     <t>collectif « Pasde0deConduite pour les enfants de 3 ans »</t>
   </si>
   <si>
@@ -846,9 +828,6 @@
 psychiatres</t>
   </si>
   <si>
-    <t>classification;médical</t>
-  </si>
-  <si>
     <t>classification:apa:dsm4</t>
   </si>
   <si>
@@ -878,9 +857,6 @@
     <t>ISBN:2738105084</t>
   </si>
   <si>
-    <t>livre;SHS</t>
-  </si>
-  <si>
     <t>Pour La Recherche, Bulletin de La Fédération Française de Psychiatrie n° 51, Décembre 2006, pp 2-7</t>
   </si>
   <si>
@@ -895,9 +871,6 @@
   </si>
   <si>
     <t>rapport:hermange:2006</t>
-  </si>
-  <si>
-    <t>Institute of Medicine of the national academies;US Institutions</t>
   </si>
   <si>
     <t>MJ</t>
@@ -1035,9 +1008,6 @@
     <t>collectif:MURS:cahiers47</t>
   </si>
   <si>
-    <t>Institution</t>
-  </si>
-  <si>
     <t>MS</t>
   </si>
   <si>
@@ -1217,12 +1187,6 @@
     <t>Code de procédure pénale</t>
   </si>
   <si>
-    <t>Convention Européenne des Droits de l'Homme</t>
-  </si>
-  <si>
-    <t>Loi UK</t>
-  </si>
-  <si>
     <t>Cette saisine a été aussi adressée au Comité d’Ethique de l’INSERM (ERMES) qui a
 rendu un rapport en date du 28 août 20071</t>
   </si>
@@ -1274,10 +1238,6 @@
     <t>Martin Hirsch;Jérôme Cordelier</t>
   </si>
   <si>
-    <t>Préambule de la Déclaration UNIVERSELLE des
-Droits de l’Homme du 10 décembre 1948</t>
-  </si>
-  <si>
     <t>B. Grenier : “Justifier les décisions médicales et maîtriser les coûts”, 4e édition,
 2006, Masson, Paris, 141 pages</t>
   </si>
@@ -1289,9 +1249,6 @@
   </si>
   <si>
     <t>ISBN:9782081428447</t>
-  </si>
-  <si>
-    <t>livre;ECO</t>
   </si>
   <si>
     <t>Bernard Grenier</t>
@@ -1376,18 +1333,12 @@
     <t>ISBN:9782070400553</t>
   </si>
   <si>
-    <t>livre;philo</t>
-  </si>
-  <si>
     <t>Jorge Semprun</t>
   </si>
   <si>
     <t xml:space="preserve">ark:/13960/s2ffk477564 </t>
   </si>
   <si>
-    <t>livre;psycho</t>
-  </si>
-  <si>
     <t>ISBN-13:978-0679772897</t>
   </si>
   <si>
@@ -1395,9 +1346,6 @@
   </si>
   <si>
     <t>urn:oclc:record:1033568750</t>
-  </si>
-  <si>
-    <t>livre;autobio</t>
   </si>
   <si>
     <t xml:space="preserve"> Jean-Dominique Bauby Le Scaphandre et le papillon. Robert Laffont. 1999.</t>
@@ -1486,15 +1434,9 @@
     <t>Charles Darwin</t>
   </si>
   <si>
-    <t>classic;psycho</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Daniel Bailly (1) , Manuel Bouvard (2) , Françoise Casadebaig (3) , Maurice Corcos (4) , Eric Fombonne (5) , Philip Gorwood (6) , Pierre Gressens (7) , Marie-Odile Krebs (8) , Marie-Thérèse Le Normand (9) , Jean-Luc Martinot (10) , Diane Ouakil-Purper (11) , Marie-Scania de Schonen (12) , Hélène Verdoux (13) </t>
   </si>
   <si>
-    <t>rapport;médical</t>
-  </si>
-  <si>
     <t>HA:hal-01570673</t>
   </si>
   <si>
@@ -1502,9 +1444,6 @@
   </si>
   <si>
     <t xml:space="preserve"> ISBN:9782700704297</t>
-  </si>
-  <si>
-    <t>classic;philo</t>
   </si>
   <si>
     <t>rapport:ccompte:06032007</t>
@@ -1592,15 +1531,6 @@
   </si>
   <si>
     <t>CPP</t>
-  </si>
-  <si>
-    <t>CEDH</t>
-  </si>
-  <si>
-    <t>loiUK</t>
-  </si>
-  <si>
-    <t>DUDH</t>
   </si>
   <si>
     <t>90;93;97;104</t>
@@ -1699,6 +1629,138 @@
   </si>
   <si>
     <t>Dreifuss-Netter F. Dossier médical et DMP. Hôpitaux magazine, 2007, n° 3, pp. 31-35</t>
+  </si>
+  <si>
+    <t>IGAS;IGF;CGT</t>
+  </si>
+  <si>
+    <t>MS;MEco</t>
+  </si>
+  <si>
+    <t>rapport:igasigfcgti;2007</t>
+  </si>
+  <si>
+    <t>avis:cnil:dmp2007</t>
+  </si>
+  <si>
+    <t>CNIL</t>
+  </si>
+  <si>
+    <t>rapport:fagniez:2007</t>
+  </si>
+  <si>
+    <t>processus législatif</t>
+  </si>
+  <si>
+    <t>procesleg:an:rapinfo0659</t>
+  </si>
+  <si>
+    <t>Espace Ethique Hopsitalier</t>
+  </si>
+  <si>
+    <t>Espace Ethique Méditerranéen de Marseille</t>
+  </si>
+  <si>
+    <t>avis:eeh:3783</t>
+  </si>
+  <si>
+    <t>rapport:gagneux:052008</t>
+  </si>
+  <si>
+    <t>Conseil national de l'Ordre des médecins</t>
+  </si>
+  <si>
+    <t>rapport:cnom:052008</t>
+  </si>
+  <si>
+    <t>ISBN:978-2-84874-032-4</t>
+  </si>
+  <si>
+    <t>Olivier Dupuis</t>
+  </si>
+  <si>
+    <t>presse spécialisée</t>
+  </si>
+  <si>
+    <t>presse:hopitalmag:032007</t>
+  </si>
+  <si>
+    <t>Hopital Mag</t>
+  </si>
+  <si>
+    <t>presse:actualitésanté:582007</t>
+  </si>
+  <si>
+    <t>Actualité et dossier en santé publique</t>
+  </si>
+  <si>
+    <t>DOI:10.3917/spub.061.0107</t>
+  </si>
+  <si>
+    <t>BNDS:2656</t>
+  </si>
+  <si>
+    <t>ISBN:978-2-84874-072-0</t>
+  </si>
+  <si>
+    <t>DOI:10.3917/lae.071.0012</t>
+  </si>
+  <si>
+    <t>article</t>
+  </si>
+  <si>
+    <t>chrétien</t>
+  </si>
+  <si>
+    <t>droit</t>
+  </si>
+  <si>
+    <t>éthique</t>
+  </si>
+  <si>
+    <t>médical</t>
+  </si>
+  <si>
+    <t>biologie</t>
+  </si>
+  <si>
+    <t>ECO</t>
+  </si>
+  <si>
+    <t>philo</t>
+  </si>
+  <si>
+    <t>autobio</t>
+  </si>
+  <si>
+    <t>psycho</t>
+  </si>
+  <si>
+    <t>SHS</t>
+  </si>
+  <si>
+    <t>Institution_Domaine</t>
+  </si>
+  <si>
+    <t>Institute of Medicine of the national academies</t>
+  </si>
+  <si>
+    <t>thèse</t>
+  </si>
+  <si>
+    <t>classification</t>
+  </si>
+  <si>
+    <t>MEco</t>
+  </si>
+  <si>
+    <t>Déclaration (Européenne/Universelle) droits de l'homme</t>
+  </si>
+  <si>
+    <t>98;101</t>
+  </si>
+  <si>
+    <t>Déclaration Droits de l'Homme</t>
   </si>
 </sst>
 </file>
@@ -2107,22 +2169,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E04038-3509-4F35-9526-D1862560050B}">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="B176" sqref="B176:B183"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="E159" sqref="E159:F159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="61.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="5" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="61.54296875" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="5" width="33.81640625" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -2133,10 +2195,10 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="E1" t="s">
-        <v>309</v>
+        <v>524</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -2148,7 +2210,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2161,14 +2223,17 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
+      <c r="E2" t="s">
+        <v>523</v>
+      </c>
       <c r="F2" t="s">
-        <v>268</v>
+        <v>7</v>
       </c>
       <c r="G2">
         <v>2001</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2181,14 +2246,17 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
+      <c r="E3" t="s">
+        <v>517</v>
+      </c>
       <c r="F3" t="s">
-        <v>247</v>
+        <v>513</v>
       </c>
       <c r="G3">
         <v>2002</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2201,14 +2269,17 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
+      <c r="E4" t="s">
+        <v>517</v>
+      </c>
       <c r="F4" t="s">
-        <v>247</v>
+        <v>513</v>
       </c>
       <c r="G4">
         <v>2003</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2222,13 +2293,13 @@
         <v>242</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>504</v>
       </c>
       <c r="G5">
         <v>2002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -2248,7 +2319,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>240</v>
       </c>
@@ -2268,7 +2339,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -2279,10 +2350,10 @@
         <v>205</v>
       </c>
       <c r="D8" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="E8" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
@@ -2294,7 +2365,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2311,13 +2382,13 @@
         <v>242</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>504</v>
       </c>
       <c r="G9">
         <v>2004</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2330,14 +2401,17 @@
       <c r="D10" t="s">
         <v>3</v>
       </c>
+      <c r="E10" t="s">
+        <v>516</v>
+      </c>
       <c r="F10" t="s">
-        <v>248</v>
+        <v>7</v>
       </c>
       <c r="G10">
         <v>1985</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2350,15 +2424,17 @@
       <c r="D11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" t="s">
+        <v>516</v>
+      </c>
       <c r="F11" t="s">
-        <v>248</v>
+        <v>7</v>
       </c>
       <c r="G11" s="2">
         <v>2001</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2371,14 +2447,17 @@
       <c r="D12" t="s">
         <v>24</v>
       </c>
+      <c r="E12" t="s">
+        <v>516</v>
+      </c>
       <c r="F12" t="s">
-        <v>248</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <v>1992</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2391,15 +2470,17 @@
       <c r="D13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" t="s">
+        <v>516</v>
+      </c>
       <c r="F13" t="s">
-        <v>248</v>
+        <v>7</v>
       </c>
       <c r="G13">
         <v>2002</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2412,14 +2493,17 @@
       <c r="D14" t="s">
         <v>30</v>
       </c>
+      <c r="E14" t="s">
+        <v>516</v>
+      </c>
       <c r="F14" t="s">
-        <v>248</v>
+        <v>7</v>
       </c>
       <c r="G14">
         <v>1999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2430,10 +2514,10 @@
         <v>207</v>
       </c>
       <c r="D15" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E15" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
@@ -2445,7 +2529,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -2459,7 +2543,7 @@
         <v>118</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>494</v>
       </c>
       <c r="G16">
         <v>2004</v>
@@ -2468,7 +2552,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2491,12 +2575,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -2514,7 +2598,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2527,14 +2611,17 @@
       <c r="D19" t="s">
         <v>48</v>
       </c>
+      <c r="E19" t="s">
+        <v>516</v>
+      </c>
       <c r="F19" t="s">
-        <v>249</v>
+        <v>513</v>
       </c>
       <c r="G19">
         <v>2004</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2557,7 +2644,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2568,10 +2655,10 @@
         <v>210</v>
       </c>
       <c r="D21" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="E21" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
@@ -2580,7 +2667,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -2603,7 +2690,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -2626,7 +2713,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -2637,10 +2724,10 @@
         <v>213</v>
       </c>
       <c r="D24" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E24" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="F24" t="s">
         <v>5</v>
@@ -2649,7 +2736,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -2669,7 +2756,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -2683,16 +2770,16 @@
         <v>64</v>
       </c>
       <c r="E26" t="s">
-        <v>64</v>
+        <v>520</v>
       </c>
       <c r="F26" t="s">
-        <v>7</v>
+        <v>419</v>
       </c>
       <c r="G26">
         <v>1670</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -2705,6 +2792,9 @@
       <c r="D27" t="s">
         <v>68</v>
       </c>
+      <c r="E27" t="s">
+        <v>520</v>
+      </c>
       <c r="F27" t="s">
         <v>7</v>
       </c>
@@ -2712,7 +2802,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -2725,6 +2815,9 @@
       <c r="D28" t="s">
         <v>71</v>
       </c>
+      <c r="E28" t="s">
+        <v>514</v>
+      </c>
       <c r="F28" t="s">
         <v>7</v>
       </c>
@@ -2732,7 +2825,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2745,6 +2838,9 @@
       <c r="D29" t="s">
         <v>70</v>
       </c>
+      <c r="E29" t="s">
+        <v>523</v>
+      </c>
       <c r="F29" t="s">
         <v>7</v>
       </c>
@@ -2752,7 +2848,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -2772,7 +2868,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -2792,7 +2888,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>80</v>
       </c>
@@ -2803,10 +2899,10 @@
         <v>217</v>
       </c>
       <c r="D32" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="E32" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="F32" t="s">
         <v>5</v>
@@ -2815,7 +2911,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>81</v>
       </c>
@@ -2826,7 +2922,7 @@
         <v>218</v>
       </c>
       <c r="E33" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="F33" t="s">
         <v>5</v>
@@ -2835,7 +2931,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>82</v>
       </c>
@@ -2855,7 +2951,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>83</v>
       </c>
@@ -2869,13 +2965,13 @@
         <v>84</v>
       </c>
       <c r="F35" t="s">
-        <v>34</v>
+        <v>494</v>
       </c>
       <c r="G35">
         <v>2001</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>85</v>
       </c>
@@ -2888,14 +2984,17 @@
       <c r="D36" t="s">
         <v>86</v>
       </c>
+      <c r="E36" t="s">
+        <v>515</v>
+      </c>
       <c r="F36" t="s">
-        <v>250</v>
+        <v>513</v>
       </c>
       <c r="G36">
         <v>2003</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -2915,7 +3014,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2926,10 +3025,10 @@
         <v>99</v>
       </c>
       <c r="D38" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="E38" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="F38" t="s">
         <v>5</v>
@@ -2938,7 +3037,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>89</v>
       </c>
@@ -2952,12 +3051,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>487</v>
+        <v>464</v>
       </c>
       <c r="C40" t="s">
         <v>92</v>
@@ -2966,7 +3065,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>93</v>
       </c>
@@ -2983,13 +3082,13 @@
         <v>178</v>
       </c>
       <c r="F41" t="s">
-        <v>34</v>
+        <v>494</v>
       </c>
       <c r="G41">
         <v>2003</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>95</v>
       </c>
@@ -2999,11 +3098,14 @@
       <c r="C42" t="s">
         <v>96</v>
       </c>
+      <c r="F42" t="s">
+        <v>34</v>
+      </c>
       <c r="G42">
         <v>1994</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -3017,7 +3119,7 @@
         <v>101</v>
       </c>
       <c r="E43" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="F43" t="s">
         <v>223</v>
@@ -3026,7 +3128,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>102</v>
       </c>
@@ -3046,7 +3148,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>104</v>
       </c>
@@ -3059,14 +3161,17 @@
       <c r="D45" t="s">
         <v>105</v>
       </c>
+      <c r="E45" t="s">
+        <v>516</v>
+      </c>
       <c r="F45" t="s">
-        <v>248</v>
+        <v>7</v>
       </c>
       <c r="G45">
         <v>1997</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -3086,7 +3191,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>109</v>
       </c>
@@ -3099,6 +3204,9 @@
       <c r="D47" t="s">
         <v>111</v>
       </c>
+      <c r="E47" t="s">
+        <v>517</v>
+      </c>
       <c r="F47" t="s">
         <v>110</v>
       </c>
@@ -3106,7 +3214,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>113</v>
       </c>
@@ -3119,19 +3227,22 @@
       <c r="D48" t="s">
         <v>114</v>
       </c>
+      <c r="E48" t="s">
+        <v>517</v>
+      </c>
       <c r="F48" t="s">
-        <v>247</v>
+        <v>513</v>
       </c>
       <c r="G48">
         <v>2002</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>116</v>
       </c>
       <c r="B49" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
       <c r="C49" t="s">
         <v>117</v>
@@ -3146,7 +3257,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>120</v>
       </c>
@@ -3166,7 +3277,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>122</v>
       </c>
@@ -3176,8 +3287,11 @@
       <c r="C51" t="s">
         <v>227</v>
       </c>
+      <c r="D51" t="s">
+        <v>525</v>
+      </c>
       <c r="E51" t="s">
-        <v>274</v>
+        <v>324</v>
       </c>
       <c r="F51" t="s">
         <v>5</v>
@@ -3186,7 +3300,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>123</v>
       </c>
@@ -3199,15 +3313,17 @@
       <c r="D52" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E52" s="4"/>
+      <c r="E52" s="4" t="s">
+        <v>513</v>
+      </c>
       <c r="F52" t="s">
-        <v>247</v>
+        <v>517</v>
       </c>
       <c r="G52">
         <v>1997</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>128</v>
       </c>
@@ -3220,15 +3336,17 @@
       <c r="D53" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E53" s="4"/>
+      <c r="E53" s="4" t="s">
+        <v>513</v>
+      </c>
       <c r="F53" t="s">
-        <v>247</v>
+        <v>517</v>
       </c>
       <c r="G53">
         <v>2000</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>130</v>
       </c>
@@ -3241,14 +3359,17 @@
       <c r="D54" t="s">
         <v>131</v>
       </c>
+      <c r="E54" s="4" t="s">
+        <v>513</v>
+      </c>
       <c r="F54" t="s">
-        <v>247</v>
+        <v>517</v>
       </c>
       <c r="G54">
         <v>2003</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>132</v>
       </c>
@@ -3261,14 +3382,17 @@
       <c r="D55" t="s">
         <v>133</v>
       </c>
+      <c r="E55" s="4" t="s">
+        <v>523</v>
+      </c>
       <c r="F55" t="s">
-        <v>251</v>
+        <v>526</v>
       </c>
       <c r="G55">
         <v>1998</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>135</v>
       </c>
@@ -3278,14 +3402,17 @@
       <c r="C56" t="s">
         <v>136</v>
       </c>
+      <c r="E56" s="4" t="s">
+        <v>517</v>
+      </c>
       <c r="F56" t="s">
-        <v>247</v>
+        <v>513</v>
       </c>
       <c r="G56">
         <v>2006</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>138</v>
       </c>
@@ -3305,7 +3432,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>170</v>
       </c>
@@ -3316,7 +3443,7 @@
         <v>230</v>
       </c>
       <c r="E58" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="F58" t="s">
         <v>51</v>
@@ -3325,7 +3452,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>173</v>
       </c>
@@ -3336,13 +3463,13 @@
         <v>231</v>
       </c>
       <c r="E59" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="F59" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>144</v>
       </c>
@@ -3356,7 +3483,7 @@
         <v>145</v>
       </c>
       <c r="E60" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="F60" t="s">
         <v>223</v>
@@ -3365,7 +3492,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>146</v>
       </c>
@@ -3375,14 +3502,17 @@
       <c r="C61" t="s">
         <v>152</v>
       </c>
+      <c r="E61" t="s">
+        <v>518</v>
+      </c>
       <c r="F61" t="s">
-        <v>252</v>
+        <v>513</v>
       </c>
       <c r="G61">
         <v>2004</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>147</v>
       </c>
@@ -3392,14 +3522,17 @@
       <c r="C62" t="s">
         <v>153</v>
       </c>
+      <c r="E62" t="s">
+        <v>518</v>
+      </c>
       <c r="F62" t="s">
-        <v>252</v>
+        <v>513</v>
       </c>
       <c r="G62">
         <v>2004</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>148</v>
       </c>
@@ -3409,14 +3542,17 @@
       <c r="C63" t="s">
         <v>149</v>
       </c>
+      <c r="E63" t="s">
+        <v>518</v>
+      </c>
       <c r="F63" t="s">
-        <v>252</v>
+        <v>513</v>
       </c>
       <c r="G63">
         <v>2005</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>150</v>
       </c>
@@ -3426,11 +3562,14 @@
       <c r="C64" t="s">
         <v>151</v>
       </c>
+      <c r="E64" t="s">
+        <v>518</v>
+      </c>
       <c r="F64" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>154</v>
       </c>
@@ -3440,11 +3579,14 @@
       <c r="C65" s="4" t="s">
         <v>160</v>
       </c>
+      <c r="E65" t="s">
+        <v>518</v>
+      </c>
       <c r="F65" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>155</v>
       </c>
@@ -3454,11 +3596,14 @@
       <c r="C66" t="s">
         <v>161</v>
       </c>
+      <c r="E66" t="s">
+        <v>518</v>
+      </c>
       <c r="F66" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>156</v>
       </c>
@@ -3468,11 +3613,14 @@
       <c r="C67" t="s">
         <v>162</v>
       </c>
+      <c r="E67" t="s">
+        <v>518</v>
+      </c>
       <c r="F67" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>157</v>
       </c>
@@ -3482,11 +3630,14 @@
       <c r="C68" t="s">
         <v>165</v>
       </c>
+      <c r="E68" t="s">
+        <v>518</v>
+      </c>
       <c r="F68" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>158</v>
       </c>
@@ -3496,11 +3647,14 @@
       <c r="C69" t="s">
         <v>164</v>
       </c>
+      <c r="E69" t="s">
+        <v>518</v>
+      </c>
       <c r="F69" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>159</v>
       </c>
@@ -3510,11 +3664,14 @@
       <c r="C70" t="s">
         <v>163</v>
       </c>
+      <c r="E70" t="s">
+        <v>518</v>
+      </c>
       <c r="F70" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>166</v>
       </c>
@@ -3524,11 +3681,14 @@
       <c r="C71" t="s">
         <v>167</v>
       </c>
+      <c r="E71" t="s">
+        <v>518</v>
+      </c>
       <c r="F71" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>168</v>
       </c>
@@ -3538,11 +3698,14 @@
       <c r="C72" t="s">
         <v>169</v>
       </c>
+      <c r="E72" t="s">
+        <v>518</v>
+      </c>
       <c r="F72" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>171</v>
       </c>
@@ -3556,7 +3719,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>198</v>
       </c>
@@ -3573,7 +3736,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>174</v>
       </c>
@@ -3590,7 +3753,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>175</v>
       </c>
@@ -3607,12 +3770,12 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>493</v>
+        <v>470</v>
       </c>
       <c r="B77" t="s">
-        <v>494</v>
+        <v>471</v>
       </c>
       <c r="C77" t="s">
         <v>202</v>
@@ -3624,7 +3787,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>176</v>
       </c>
@@ -3641,7 +3804,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>177</v>
       </c>
@@ -3655,13 +3818,13 @@
         <v>178</v>
       </c>
       <c r="F79" t="s">
-        <v>34</v>
+        <v>494</v>
       </c>
       <c r="G79">
         <v>2000</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>179</v>
       </c>
@@ -3675,13 +3838,13 @@
         <v>84</v>
       </c>
       <c r="F80" t="s">
-        <v>34</v>
+        <v>494</v>
       </c>
       <c r="G80">
         <v>2000</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>180</v>
       </c>
@@ -3695,7 +3858,7 @@
         <v>181</v>
       </c>
       <c r="E81" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="F81" t="s">
         <v>5</v>
@@ -3704,7 +3867,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>182</v>
       </c>
@@ -3724,7 +3887,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>183</v>
       </c>
@@ -3744,7 +3907,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>184</v>
       </c>
@@ -3761,7 +3924,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>185</v>
       </c>
@@ -3781,7 +3944,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>187</v>
       </c>
@@ -3801,7 +3964,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>188</v>
       </c>
@@ -3812,10 +3975,10 @@
         <v>197</v>
       </c>
       <c r="D87" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="E87" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="F87" t="s">
         <v>189</v>
@@ -3824,7 +3987,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>190</v>
       </c>
@@ -3838,7 +4001,7 @@
         <v>191</v>
       </c>
       <c r="E88" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="F88" t="s">
         <v>5</v>
@@ -3847,7 +4010,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>193</v>
       </c>
@@ -3858,10 +4021,10 @@
         <v>194</v>
       </c>
       <c r="D89" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="E89" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="F89" t="s">
         <v>5</v>
@@ -3870,7 +4033,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>195</v>
       </c>
@@ -3881,7 +4044,7 @@
         <v>196</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>56</v>
@@ -3893,75 +4056,75 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B91">
         <v>95</v>
       </c>
       <c r="C91" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D91" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E91" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F91" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B92">
         <v>95</v>
       </c>
       <c r="C92" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D92" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="E92" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="F92" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B93">
         <v>95</v>
       </c>
       <c r="C93" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E93" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="F93" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B94">
         <v>95</v>
       </c>
       <c r="C94" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E94" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="F94" t="s">
         <v>5</v>
@@ -3970,61 +4133,67 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B95">
         <v>95</v>
       </c>
       <c r="C95" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D95" t="s">
-        <v>266</v>
+        <v>259</v>
+      </c>
+      <c r="E95" t="s">
+        <v>523</v>
       </c>
       <c r="F95" t="s">
-        <v>268</v>
+        <v>7</v>
       </c>
       <c r="G95">
         <v>1997</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B96">
         <v>95</v>
       </c>
       <c r="C96" t="s">
-        <v>271</v>
+        <v>263</v>
+      </c>
+      <c r="D96" t="s">
+        <v>262</v>
       </c>
       <c r="E96" t="s">
-        <v>270</v>
+        <v>517</v>
       </c>
       <c r="F96" t="s">
-        <v>247</v>
+        <v>513</v>
       </c>
       <c r="G96">
         <v>2006</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B97">
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D97" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="E97" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="F97" t="s">
         <v>5</v>
@@ -4033,58 +4202,61 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="B98">
         <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>279</v>
+        <v>270</v>
+      </c>
+      <c r="E98" t="s">
+        <v>518</v>
       </c>
       <c r="F98" t="s">
-        <v>252</v>
+        <v>513</v>
       </c>
       <c r="G98">
         <v>2006</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B99">
         <v>95</v>
       </c>
       <c r="C99" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D99" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="E99" t="s">
-        <v>282</v>
+        <v>523</v>
       </c>
       <c r="F99" t="s">
-        <v>268</v>
+        <v>7</v>
       </c>
       <c r="G99">
         <v>2000</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B100">
         <v>95</v>
       </c>
       <c r="C100" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="E100" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="F100" t="s">
         <v>5</v>
@@ -4093,18 +4265,18 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B101">
         <v>96</v>
       </c>
       <c r="C101" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="E101" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="F101" t="s">
         <v>5</v>
@@ -4113,18 +4285,18 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B102">
         <v>96</v>
       </c>
       <c r="C102" t="s">
+        <v>297</v>
+      </c>
+      <c r="E102" t="s">
         <v>306</v>
-      </c>
-      <c r="E102" t="s">
-        <v>316</v>
       </c>
       <c r="F102" t="s">
         <v>51</v>
@@ -4133,38 +4305,41 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B103">
         <v>96</v>
       </c>
       <c r="C103" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="E103" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="F103" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="G103">
         <v>2006</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B104">
         <v>96</v>
       </c>
       <c r="C104" t="s">
-        <v>323</v>
+        <v>313</v>
+      </c>
+      <c r="D104" t="s">
+        <v>312</v>
       </c>
       <c r="E104" t="s">
-        <v>322</v>
+        <v>528</v>
       </c>
       <c r="F104" t="s">
         <v>5</v>
@@ -4173,18 +4348,18 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B105">
         <v>96</v>
       </c>
       <c r="C105" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="E105" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="F105" t="s">
         <v>5</v>
@@ -4193,18 +4368,18 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B106">
         <v>96</v>
       </c>
       <c r="C106" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="E106" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="F106" t="s">
         <v>5</v>
@@ -4213,35 +4388,35 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B107">
         <v>96</v>
       </c>
       <c r="C107" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="E107" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="F107" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B108">
         <v>96</v>
       </c>
       <c r="C108" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E108" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="F108" t="s">
         <v>5</v>
@@ -4250,18 +4425,18 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B109">
         <v>96</v>
       </c>
       <c r="C109" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="E109" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="F109" t="s">
         <v>5</v>
@@ -4270,18 +4445,18 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B110">
         <v>96</v>
       </c>
       <c r="C110" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="E110" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="F110" t="s">
         <v>5</v>
@@ -4290,18 +4465,18 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B111">
         <v>96</v>
       </c>
       <c r="C111" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="E111" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="F111" t="s">
         <v>34</v>
@@ -4310,18 +4485,18 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B112">
         <v>96</v>
       </c>
       <c r="C112" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="D112" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="E112" t="s">
         <v>62</v>
@@ -4333,18 +4508,18 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B113">
         <v>96</v>
       </c>
       <c r="C113" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="E113" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="F113" t="s">
         <v>5</v>
@@ -4353,18 +4528,18 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B114">
         <v>96</v>
       </c>
       <c r="C114" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="E114" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F114" t="s">
         <v>5</v>
@@ -4373,18 +4548,18 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B115">
         <v>96</v>
       </c>
       <c r="C115" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="E115" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="F115" t="s">
         <v>51</v>
@@ -4393,64 +4568,64 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B116">
         <v>96</v>
       </c>
       <c r="C116" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="E116" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="F116" t="s">
-        <v>34</v>
+        <v>494</v>
       </c>
       <c r="G116">
         <v>2006</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B117">
         <v>96</v>
       </c>
       <c r="C117" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="D117" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="E117" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F117" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="G117">
         <v>2003</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B118">
         <v>96</v>
       </c>
       <c r="C118" t="s">
-        <v>482</v>
+        <v>462</v>
       </c>
       <c r="D118" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="E118" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="F118" t="s">
         <v>5</v>
@@ -4459,988 +4634,1155 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B119">
         <v>97</v>
       </c>
       <c r="C119" t="s">
-        <v>360</v>
+        <v>350</v>
+      </c>
+      <c r="E119" t="s">
+        <v>517</v>
       </c>
       <c r="F119" t="s">
-        <v>247</v>
+        <v>513</v>
       </c>
       <c r="G119">
         <v>2006</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B120">
         <v>97</v>
       </c>
       <c r="C120" t="s">
-        <v>361</v>
+        <v>351</v>
+      </c>
+      <c r="E120" t="s">
+        <v>517</v>
       </c>
       <c r="F120" t="s">
-        <v>247</v>
+        <v>513</v>
       </c>
       <c r="G120">
         <v>2005</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B121">
         <v>98</v>
       </c>
       <c r="C121" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="D121" t="s">
-        <v>363</v>
+        <v>353</v>
+      </c>
+      <c r="E121" t="s">
+        <v>516</v>
       </c>
       <c r="F121" t="s">
-        <v>248</v>
+        <v>7</v>
       </c>
       <c r="G121">
         <v>1990</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="B122">
         <v>98</v>
       </c>
       <c r="C122" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="D122" t="s">
-        <v>367</v>
+        <v>357</v>
+      </c>
+      <c r="E122" t="s">
+        <v>516</v>
       </c>
       <c r="F122" t="s">
-        <v>248</v>
+        <v>7</v>
       </c>
       <c r="G122">
         <v>2007</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B123">
         <v>98</v>
       </c>
       <c r="C123" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+      <c r="F123" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>369</v>
-      </c>
-      <c r="B124">
-        <v>98</v>
-      </c>
-      <c r="C124" t="s">
-        <v>484</v>
+        <v>529</v>
+      </c>
+      <c r="B124" t="s">
+        <v>530</v>
+      </c>
+      <c r="E124" t="s">
+        <v>531</v>
       </c>
       <c r="F124" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="B125">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C125" t="s">
-        <v>485</v>
+        <v>361</v>
       </c>
       <c r="E125" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+      <c r="F125" t="s">
+        <v>51</v>
+      </c>
+      <c r="G125">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="B126">
         <v>99</v>
       </c>
       <c r="C126" t="s">
-        <v>373</v>
-      </c>
-      <c r="E126" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F126" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="G126">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="B127">
         <v>99</v>
       </c>
       <c r="C127" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="F127" t="s">
         <v>34</v>
       </c>
       <c r="G127">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="B128">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C128" t="s">
-        <v>378</v>
+        <v>369</v>
+      </c>
+      <c r="E128" t="s">
+        <v>368</v>
       </c>
       <c r="F128" t="s">
-        <v>34</v>
-      </c>
-      <c r="G128">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B129">
         <v>101</v>
       </c>
       <c r="C129" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="E129" t="s">
-        <v>380</v>
+        <v>245</v>
       </c>
       <c r="F129" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G129">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="B130">
         <v>101</v>
       </c>
       <c r="C130" t="s">
-        <v>383</v>
+        <v>373</v>
+      </c>
+      <c r="D130" t="s">
+        <v>374</v>
       </c>
       <c r="E130" t="s">
-        <v>245</v>
+        <v>523</v>
       </c>
       <c r="F130" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G130">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="B131">
         <v>101</v>
       </c>
       <c r="C131" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D131" t="s">
-        <v>386</v>
+        <v>379</v>
+      </c>
+      <c r="E131" t="s">
+        <v>519</v>
       </c>
       <c r="F131" t="s">
-        <v>268</v>
+        <v>7</v>
       </c>
       <c r="G131">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="B132">
         <v>101</v>
       </c>
       <c r="C132" t="s">
-        <v>486</v>
+        <v>378</v>
+      </c>
+      <c r="D132" t="s">
+        <v>377</v>
+      </c>
+      <c r="E132" t="s">
+        <v>519</v>
+      </c>
+      <c r="F132" t="s">
+        <v>7</v>
       </c>
       <c r="G132">
-        <v>1948</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B133">
         <v>101</v>
       </c>
       <c r="C133" t="s">
-        <v>394</v>
-      </c>
-      <c r="D133" t="s">
-        <v>393</v>
+        <v>382</v>
+      </c>
+      <c r="E133" t="s">
+        <v>245</v>
       </c>
       <c r="F133" t="s">
-        <v>392</v>
-      </c>
-      <c r="G133">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="B134">
         <v>101</v>
       </c>
       <c r="C134" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="D134" t="s">
-        <v>390</v>
+        <v>384</v>
+      </c>
+      <c r="E134" t="s">
+        <v>300</v>
       </c>
       <c r="F134" t="s">
-        <v>392</v>
-      </c>
-      <c r="G134">
-        <v>1863</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="B135">
         <v>101</v>
       </c>
       <c r="C135" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="E135" t="s">
-        <v>245</v>
+        <v>523</v>
       </c>
       <c r="F135" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="B136">
         <v>101</v>
       </c>
       <c r="C136" t="s">
-        <v>399</v>
-      </c>
-      <c r="D136" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="E136" t="s">
-        <v>310</v>
+        <v>390</v>
       </c>
       <c r="F136" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="B137">
         <v>101</v>
       </c>
       <c r="C137" t="s">
-        <v>401</v>
+        <v>395</v>
+      </c>
+      <c r="E137" t="s">
+        <v>36</v>
       </c>
       <c r="F137" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="B138">
         <v>101</v>
       </c>
       <c r="C138" t="s">
-        <v>403</v>
+        <v>396</v>
+      </c>
+      <c r="D138" t="s">
+        <v>397</v>
       </c>
       <c r="E138" t="s">
-        <v>404</v>
+        <v>516</v>
       </c>
       <c r="F138" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="B139">
         <v>101</v>
       </c>
       <c r="C139" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="E139" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="F139" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="B140">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C140" t="s">
-        <v>410</v>
-      </c>
-      <c r="D140" t="s">
-        <v>411</v>
+        <v>404</v>
+      </c>
+      <c r="E140" t="s">
+        <v>522</v>
       </c>
       <c r="F140" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B141">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C141" t="s">
-        <v>407</v>
+        <v>402</v>
+      </c>
+      <c r="D141" t="s">
+        <v>403</v>
       </c>
       <c r="E141" t="s">
-        <v>56</v>
+        <v>520</v>
       </c>
       <c r="F141" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="B142">
         <v>102</v>
       </c>
       <c r="C142" t="s">
-        <v>419</v>
+        <v>405</v>
+      </c>
+      <c r="D142" t="s">
+        <v>406</v>
+      </c>
+      <c r="E142" t="s">
+        <v>521</v>
       </c>
       <c r="F142" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A143" s="4" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="B143">
         <v>102</v>
       </c>
-      <c r="C143" t="s">
-        <v>416</v>
+      <c r="C143" s="1" t="s">
+        <v>407</v>
       </c>
       <c r="D143" t="s">
-        <v>418</v>
+        <v>406</v>
+      </c>
+      <c r="E143" t="s">
+        <v>521</v>
       </c>
       <c r="F143" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" s="4" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="B144">
         <v>102</v>
       </c>
       <c r="C144" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="D144" t="s">
-        <v>422</v>
+        <v>428</v>
+      </c>
+      <c r="E144" t="s">
+        <v>521</v>
       </c>
       <c r="F144" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A145" s="4" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="B145">
         <v>102</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>423</v>
+      <c r="C145" t="s">
+        <v>429</v>
       </c>
       <c r="D145" t="s">
-        <v>422</v>
+        <v>430</v>
+      </c>
+      <c r="E145" t="s">
+        <v>522</v>
       </c>
       <c r="F145" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A146" s="4" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="B146">
         <v>102</v>
       </c>
       <c r="C146" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="D146" t="s">
-        <v>445</v>
+        <v>433</v>
+      </c>
+      <c r="E146" t="s">
+        <v>255</v>
       </c>
       <c r="F146" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A147" s="4" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="B147">
         <v>102</v>
       </c>
       <c r="C147" t="s">
-        <v>446</v>
-      </c>
-      <c r="D147" t="s">
-        <v>447</v>
+        <v>435</v>
+      </c>
+      <c r="E147" t="s">
+        <v>517</v>
       </c>
       <c r="F147" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A148" s="4" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="B148">
         <v>102</v>
       </c>
       <c r="C148" t="s">
-        <v>453</v>
-      </c>
-      <c r="D148" t="s">
-        <v>451</v>
+        <v>413</v>
       </c>
       <c r="E148" t="s">
-        <v>262</v>
+        <v>360</v>
       </c>
       <c r="F148" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="4" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="B149">
         <v>102</v>
       </c>
       <c r="C149" t="s">
-        <v>454</v>
+        <v>436</v>
+      </c>
+      <c r="D149" t="s">
+        <v>431</v>
+      </c>
+      <c r="E149" t="s">
+        <v>520</v>
       </c>
       <c r="F149" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="4" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="B150">
         <v>102</v>
       </c>
       <c r="C150" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="E150" t="s">
-        <v>372</v>
+        <v>245</v>
       </c>
       <c r="F150" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A151" s="4" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="B151">
         <v>102</v>
       </c>
       <c r="C151" t="s">
-        <v>455</v>
+        <v>418</v>
       </c>
       <c r="D151" t="s">
-        <v>448</v>
+        <v>432</v>
       </c>
       <c r="F151" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A152" s="4" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="B152">
         <v>102</v>
       </c>
       <c r="C152" t="s">
-        <v>433</v>
+        <v>437</v>
+      </c>
+      <c r="E152" t="s">
+        <v>108</v>
       </c>
       <c r="F152" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="4" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="B153">
         <v>102</v>
       </c>
       <c r="C153" t="s">
-        <v>435</v>
-      </c>
-      <c r="D153" t="s">
-        <v>449</v>
+        <v>440</v>
+      </c>
+      <c r="E153" t="s">
+        <v>519</v>
       </c>
       <c r="F153" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A154" s="4" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="B154">
         <v>102</v>
       </c>
       <c r="C154" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="E154" t="s">
-        <v>108</v>
+        <v>518</v>
       </c>
       <c r="F154" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A155" s="4" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="B155">
         <v>102</v>
       </c>
       <c r="C155" t="s">
-        <v>460</v>
+        <v>442</v>
+      </c>
+      <c r="E155" t="s">
+        <v>518</v>
       </c>
       <c r="F155" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A156" s="4" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="B156">
         <v>102</v>
       </c>
-      <c r="C156" t="s">
-        <v>461</v>
+      <c r="C156" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D156" t="s">
+        <v>426</v>
+      </c>
+      <c r="E156" t="s">
+        <v>518</v>
       </c>
       <c r="F156" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A157" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B157">
         <v>102</v>
       </c>
       <c r="C157" t="s">
-        <v>462</v>
+        <v>439</v>
+      </c>
+      <c r="E157" t="s">
+        <v>518</v>
       </c>
       <c r="F157" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A158" s="4" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B158">
-        <v>102</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="D158" t="s">
-        <v>443</v>
+        <v>103</v>
+      </c>
+      <c r="C158" t="s">
+        <v>445</v>
+      </c>
+      <c r="E158" t="s">
+        <v>444</v>
       </c>
       <c r="F158" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A159" s="4" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="B159">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C159" t="s">
-        <v>459</v>
+        <v>457</v>
+      </c>
+      <c r="E159" t="s">
+        <v>516</v>
       </c>
       <c r="F159" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A160" s="4" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="B160">
         <v>103</v>
       </c>
       <c r="C160" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="E160" t="s">
-        <v>464</v>
+        <v>303</v>
       </c>
       <c r="F160" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A161" s="4" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="B161">
         <v>103</v>
       </c>
       <c r="C161" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+      <c r="D161" t="s">
+        <v>451</v>
+      </c>
+      <c r="E161" t="s">
+        <v>242</v>
+      </c>
+      <c r="F161" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A162" s="4" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="B162">
         <v>103</v>
       </c>
       <c r="C162" t="s">
-        <v>468</v>
-      </c>
-      <c r="E162" t="s">
-        <v>313</v>
+        <v>455</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>454</v>
       </c>
       <c r="F162" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A163" s="4" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="B163">
         <v>103</v>
       </c>
       <c r="C163" t="s">
-        <v>470</v>
-      </c>
-      <c r="D163" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="E163" t="s">
-        <v>242</v>
+        <v>517</v>
       </c>
       <c r="F163" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A164" s="4" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="B164">
         <v>103</v>
       </c>
       <c r="C164" t="s">
-        <v>475</v>
-      </c>
-      <c r="D164" s="4" t="s">
-        <v>474</v>
+        <v>461</v>
+      </c>
+      <c r="D164" t="s">
+        <v>459</v>
+      </c>
+      <c r="E164" t="s">
+        <v>460</v>
       </c>
       <c r="F164" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="4" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="B165">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C165" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="F165" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="4" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="B166">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C166" t="s">
-        <v>481</v>
-      </c>
-      <c r="D166" t="s">
-        <v>479</v>
-      </c>
-      <c r="E166" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="F166" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A167" s="4" t="s">
-        <v>488</v>
+        <v>472</v>
       </c>
       <c r="B167">
         <v>104</v>
       </c>
       <c r="C167" t="s">
-        <v>489</v>
+        <v>473</v>
       </c>
       <c r="F167" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A168" s="4" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
       <c r="B168">
         <v>104</v>
       </c>
       <c r="C168" t="s">
-        <v>491</v>
+        <v>490</v>
+      </c>
+      <c r="D168" t="s">
+        <v>488</v>
+      </c>
+      <c r="E168" t="s">
+        <v>489</v>
       </c>
       <c r="F168" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A169" s="4" t="s">
-        <v>495</v>
+        <v>475</v>
       </c>
       <c r="B169">
         <v>104</v>
       </c>
       <c r="C169" t="s">
-        <v>496</v>
+        <v>491</v>
+      </c>
+      <c r="E169" t="s">
+        <v>492</v>
       </c>
       <c r="F169" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A170" s="4" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="B170">
         <v>104</v>
       </c>
+      <c r="C170" t="s">
+        <v>493</v>
+      </c>
+      <c r="E170" t="s">
+        <v>300</v>
+      </c>
       <c r="F170" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A171" s="4" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
       <c r="B171">
         <v>104</v>
       </c>
+      <c r="C171" t="s">
+        <v>495</v>
+      </c>
+      <c r="E171" t="s">
+        <v>84</v>
+      </c>
       <c r="F171" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A172" s="4" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
       <c r="B172">
         <v>104</v>
       </c>
+      <c r="C172" t="s">
+        <v>498</v>
+      </c>
+      <c r="D172" t="s">
+        <v>497</v>
+      </c>
+      <c r="E172" t="s">
+        <v>496</v>
+      </c>
       <c r="F172" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A173" s="4" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
       <c r="B173">
         <v>104</v>
       </c>
+      <c r="C173" t="s">
+        <v>499</v>
+      </c>
+      <c r="E173" t="s">
+        <v>300</v>
+      </c>
       <c r="F173" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A174" s="4" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
       <c r="B174">
         <v>104</v>
       </c>
+      <c r="C174" t="s">
+        <v>501</v>
+      </c>
+      <c r="E174" t="s">
+        <v>500</v>
+      </c>
       <c r="F174" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A175" s="4" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
       <c r="B175">
         <v>104</v>
       </c>
+      <c r="C175" t="s">
+        <v>502</v>
+      </c>
+      <c r="D175" t="s">
+        <v>503</v>
+      </c>
+      <c r="E175" t="s">
+        <v>515</v>
+      </c>
       <c r="F175" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A176" s="4" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
       <c r="B176">
         <v>104</v>
       </c>
+      <c r="C176" t="s">
+        <v>509</v>
+      </c>
+      <c r="E176" t="s">
+        <v>516</v>
+      </c>
       <c r="F176" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A177" s="4" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
       <c r="B177">
         <v>104</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
+        <v>510</v>
+      </c>
+      <c r="E177" t="s">
+        <v>515</v>
+      </c>
+      <c r="F177" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A178" s="4" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="B178">
         <v>104</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C178" t="s">
+        <v>511</v>
+      </c>
+      <c r="E178" t="s">
+        <v>515</v>
+      </c>
+      <c r="F178" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A179" s="4" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
       <c r="B179">
         <v>104</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="C179" t="s">
+        <v>512</v>
+      </c>
+      <c r="E179" t="s">
+        <v>514</v>
+      </c>
+      <c r="F179" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A180" s="4" t="s">
-        <v>507</v>
+        <v>486</v>
       </c>
       <c r="B180">
         <v>104</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C180" t="s">
+        <v>507</v>
+      </c>
+      <c r="E180" t="s">
+        <v>508</v>
+      </c>
+      <c r="F180" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="4" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
       <c r="B181">
         <v>104</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A182" s="4" t="s">
-        <v>509</v>
-      </c>
-      <c r="B182">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A183" s="4" t="s">
-        <v>510</v>
-      </c>
-      <c r="B183">
-        <v>104</v>
+      <c r="C181" t="s">
+        <v>505</v>
+      </c>
+      <c r="E181" t="s">
+        <v>506</v>
+      </c>
+      <c r="F181" t="s">
+        <v>504</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" display="https://gallica.bnf.fr/ark:/12148/bpt6k33779401" xr:uid="{BDA8077D-D037-496B-9BB1-7036492E3274}"/>
     <hyperlink ref="H20" r:id="rId2" xr:uid="{C73BF169-2BED-4482-AF9B-97E60D736953}"/>
-    <hyperlink ref="C145" r:id="rId3" display="https://archive.org/search.php?query=external-identifier%3A%22urn%3Aoclc%3Arecord%3A1033568750%22" xr:uid="{DB8B71D7-2DF5-47BB-A83F-DD6CE77F939C}"/>
-    <hyperlink ref="C158" r:id="rId4" display="https://doi.org/10.1016/j.tins.2006.05.010" xr:uid="{539A429A-EC4B-4E18-8E31-82C919D75EC4}"/>
+    <hyperlink ref="C143" r:id="rId3" display="https://archive.org/search.php?query=external-identifier%3A%22urn%3Aoclc%3Arecord%3A1033568750%22" xr:uid="{DB8B71D7-2DF5-47BB-A83F-DD6CE77F939C}"/>
+    <hyperlink ref="C156" r:id="rId4" display="https://doi.org/10.1016/j.tins.2006.05.010" xr:uid="{539A429A-EC4B-4E18-8E31-82C919D75EC4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>